<commit_message>
Commit after question 2 of task 1
</commit_message>
<xml_diff>
--- a/week2/data.xlsx
+++ b/week2/data.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ider.E\Desktop\PythonCourse\Lecture 2\repo2\week2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ider.E\Desktop\PythonCourse\Lecture2\repo2\week2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79F539F-EFCA-4218-B83D-CD7C6002841E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329E375E-BED9-4994-9EE4-15A6A3E4F897}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{489879BE-C2A9-4EAA-8795-529B20F48590}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="147">
   <si>
     <t>Suren</t>
   </si>
@@ -148,6 +148,324 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>bold</t>
+  </si>
+  <si>
+    <t>Dulam</t>
+  </si>
+  <si>
+    <t>Tsenguun</t>
+  </si>
+  <si>
+    <t>Naraa</t>
+  </si>
+  <si>
+    <t>Enku</t>
+  </si>
+  <si>
+    <t>Sodoo</t>
+  </si>
+  <si>
+    <t>Uuganaa</t>
+  </si>
+  <si>
+    <t>Bayraa</t>
+  </si>
+  <si>
+    <t>Batbayar</t>
+  </si>
+  <si>
+    <t>Bayrchimeg</t>
+  </si>
+  <si>
+    <t>Zulaa</t>
+  </si>
+  <si>
+    <t>Sarangoo</t>
+  </si>
+  <si>
+    <t>Baigali</t>
+  </si>
+  <si>
+    <t>Baatar</t>
+  </si>
+  <si>
+    <t>Urnaa</t>
+  </si>
+  <si>
+    <t>Bilguun</t>
+  </si>
+  <si>
+    <t>Mandah</t>
+  </si>
+  <si>
+    <t>Jargal</t>
+  </si>
+  <si>
+    <t>Setsen</t>
+  </si>
+  <si>
+    <t>Tselmeg</t>
+  </si>
+  <si>
+    <t>Tuvshuu</t>
+  </si>
+  <si>
+    <t>Tsolmon</t>
+  </si>
+  <si>
+    <t>Delger</t>
+  </si>
+  <si>
+    <t>Munkhu</t>
+  </si>
+  <si>
+    <t>Zaya</t>
+  </si>
+  <si>
+    <t>Anu</t>
+  </si>
+  <si>
+    <t>Tamir</t>
+  </si>
+  <si>
+    <t>Chinguun</t>
+  </si>
+  <si>
+    <t>Tulga</t>
+  </si>
+  <si>
+    <t>Turuu</t>
+  </si>
+  <si>
+    <t>Batsaihan</t>
+  </si>
+  <si>
+    <t>Bold</t>
+  </si>
+  <si>
+    <t>Sanchir</t>
+  </si>
+  <si>
+    <t>Zoloo</t>
+  </si>
+  <si>
+    <t>Uyanga</t>
+  </si>
+  <si>
+    <t>Erdene</t>
+  </si>
+  <si>
+    <t>Hadhuu</t>
+  </si>
+  <si>
+    <t>Saranjav</t>
+  </si>
+  <si>
+    <t>Ragchaa</t>
+  </si>
+  <si>
+    <t>Jav</t>
+  </si>
+  <si>
+    <t>Garav</t>
+  </si>
+  <si>
+    <t>Bayan</t>
+  </si>
+  <si>
+    <t>Sainhuu</t>
+  </si>
+  <si>
+    <t>Mygmar</t>
+  </si>
+  <si>
+    <t>Temdegle</t>
+  </si>
+  <si>
+    <t>Baasandorj</t>
+  </si>
+  <si>
+    <t>Sodhuu</t>
+  </si>
+  <si>
+    <t>Meg</t>
+  </si>
+  <si>
+    <t>Ayur</t>
+  </si>
+  <si>
+    <t>Gongor</t>
+  </si>
+  <si>
+    <t>Dari</t>
+  </si>
+  <si>
+    <t>Saihan</t>
+  </si>
+  <si>
+    <t>Bileg</t>
+  </si>
+  <si>
+    <t>Otgoo</t>
+  </si>
+  <si>
+    <t>Bathuu</t>
+  </si>
+  <si>
+    <t>Tushig</t>
+  </si>
+  <si>
+    <t>Gonchig</t>
+  </si>
+  <si>
+    <t>Mygaa</t>
+  </si>
+  <si>
+    <t>Gun</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Maral</t>
+  </si>
+  <si>
+    <t>Dorj</t>
+  </si>
+  <si>
+    <t>Bathishig</t>
+  </si>
+  <si>
+    <t>DV22</t>
+  </si>
+  <si>
+    <t>GM22</t>
+  </si>
+  <si>
+    <t>MA34</t>
+  </si>
+  <si>
+    <t>NV41</t>
+  </si>
+  <si>
+    <t>AV38</t>
+  </si>
+  <si>
+    <t>UN26</t>
+  </si>
+  <si>
+    <t>OU39</t>
+  </si>
+  <si>
+    <t>AR29</t>
+  </si>
+  <si>
+    <t>AE28</t>
+  </si>
+  <si>
+    <t>RJ32</t>
+  </si>
+  <si>
+    <t>GU11</t>
+  </si>
+  <si>
+    <t>AG22</t>
+  </si>
+  <si>
+    <t>OR34</t>
+  </si>
+  <si>
+    <t>IM41</t>
+  </si>
+  <si>
+    <t>RN38</t>
+  </si>
+  <si>
+    <t>AR26</t>
+  </si>
+  <si>
+    <t>NI29</t>
+  </si>
+  <si>
+    <t>HN19</t>
+  </si>
+  <si>
+    <t>LN28</t>
+  </si>
+  <si>
+    <t>NG21</t>
+  </si>
+  <si>
+    <t>GI25</t>
+  </si>
+  <si>
+    <t>UO27</t>
+  </si>
+  <si>
+    <t>NR49</t>
+  </si>
+  <si>
+    <t>RN46</t>
+  </si>
+  <si>
+    <t>LU33</t>
+  </si>
+  <si>
+    <t>UG31</t>
+  </si>
+  <si>
+    <t>AN39</t>
+  </si>
+  <si>
+    <t>UI24</t>
+  </si>
+  <si>
+    <t>RG23</t>
+  </si>
+  <si>
+    <t>NR35</t>
+  </si>
+  <si>
+    <t>AH23</t>
+  </si>
+  <si>
+    <t>UN25</t>
+  </si>
+  <si>
+    <t>NA47</t>
+  </si>
+  <si>
+    <t>DN49</t>
+  </si>
+  <si>
+    <t>RL36</t>
+  </si>
+  <si>
+    <t>ON33</t>
+  </si>
+  <si>
+    <t>AL31</t>
+  </si>
+  <si>
+    <t>EB29</t>
+  </si>
+  <si>
+    <t>GG34</t>
+  </si>
+  <si>
+    <t>UJ33</t>
+  </si>
+  <si>
+    <t>Poltical view</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Left</t>
   </si>
 </sst>
 </file>
@@ -183,9 +501,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,22 +821,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41835BD0-3C82-408D-8043-3A3A247760FB}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52:J57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B1" t="s">
@@ -542,9 +864,12 @@
       <c r="I1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="J1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -571,9 +896,12 @@
       <c r="I2" s="1">
         <v>43964</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="J2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -600,9 +928,12 @@
       <c r="I3" s="1">
         <v>40736</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="J3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -629,9 +960,12 @@
       <c r="I4" s="1">
         <v>42900</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="J4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -658,9 +992,12 @@
       <c r="I5" s="1">
         <v>43784</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="J5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -687,9 +1024,12 @@
       <c r="I6" s="1">
         <v>41299</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="J6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -716,9 +1056,12 @@
       <c r="I7" s="1">
         <v>43163</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="J7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -745,9 +1088,12 @@
       <c r="I8" s="1">
         <v>42882</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="J8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -774,9 +1120,12 @@
       <c r="I9" s="1">
         <v>42202</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="J9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -803,9 +1152,12 @@
       <c r="I10" s="1">
         <v>43681</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="J10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -831,6 +1183,1449 @@
       </c>
       <c r="I11" s="1">
         <v>44013</v>
+      </c>
+      <c r="J11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12">
+        <f>E2+3</f>
+        <v>21</v>
+      </c>
+      <c r="F12">
+        <f>F2+1</f>
+        <v>1.5</v>
+      </c>
+      <c r="G12">
+        <f>G2+0.5</f>
+        <v>2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="1">
+        <f>I2+360</f>
+        <v>44324</v>
+      </c>
+      <c r="J12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ref="E13:E21" si="0">E3+3</f>
+        <v>26</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ref="F13:F21" si="1">F3+1</f>
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ref="G13:G21" si="2">G3+0.5</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" ref="I13:I21" si="3">I3+360</f>
+        <v>41096</v>
+      </c>
+      <c r="J13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>2.4</v>
+      </c>
+      <c r="H14" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="3"/>
+        <v>43260</v>
+      </c>
+      <c r="J14" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>2.1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="3"/>
+        <v>44144</v>
+      </c>
+      <c r="J15" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>2.8</v>
+      </c>
+      <c r="H16" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="3"/>
+        <v>41659</v>
+      </c>
+      <c r="J16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>2.6</v>
+      </c>
+      <c r="H17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="3"/>
+        <v>43523</v>
+      </c>
+      <c r="J17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" t="s">
+        <v>110</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>2.29</v>
+      </c>
+      <c r="H18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="3"/>
+        <v>43242</v>
+      </c>
+      <c r="J18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>2.9</v>
+      </c>
+      <c r="H19" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="3"/>
+        <v>42562</v>
+      </c>
+      <c r="J19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>1.8</v>
+      </c>
+      <c r="H20" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="3"/>
+        <v>44041</v>
+      </c>
+      <c r="J20" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <f>G11+0.5</f>
+        <v>2</v>
+      </c>
+      <c r="H21" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="3"/>
+        <v>44373</v>
+      </c>
+      <c r="J21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22">
+        <f>E2-2</f>
+        <v>16</v>
+      </c>
+      <c r="F22">
+        <f>F2</f>
+        <v>0.5</v>
+      </c>
+      <c r="G22">
+        <f>G2-0.5</f>
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="1">
+        <f>I2-150</f>
+        <v>43814</v>
+      </c>
+      <c r="J22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ref="E23:E34" si="4">E3-2</f>
+        <v>21</v>
+      </c>
+      <c r="F23">
+        <f>F2+0.5</f>
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23:G31" si="5">G3-0.5</f>
+        <v>1.2</v>
+      </c>
+      <c r="H23" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" ref="I23:I32" si="6">I3-150</f>
+        <v>40586</v>
+      </c>
+      <c r="J23" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" t="s">
+        <v>116</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="F24">
+        <f t="shared" ref="F24:F32" si="7">F3+0.5</f>
+        <v>2.5</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>1.4</v>
+      </c>
+      <c r="H24" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="6"/>
+        <v>42750</v>
+      </c>
+      <c r="J24" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" t="s">
+        <v>117</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="7"/>
+        <v>4.5</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="6"/>
+        <v>43634</v>
+      </c>
+      <c r="J25" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" t="s">
+        <v>118</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="5"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="H26" t="s">
+        <v>30</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="6"/>
+        <v>41149</v>
+      </c>
+      <c r="J26" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" t="s">
+        <v>119</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="7"/>
+        <v>8.5</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="5"/>
+        <v>1.6</v>
+      </c>
+      <c r="H27" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="6"/>
+        <v>43013</v>
+      </c>
+      <c r="J27" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="7"/>
+        <v>3.5</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="5"/>
+        <v>1.29</v>
+      </c>
+      <c r="H28" t="s">
+        <v>30</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="6"/>
+        <v>42732</v>
+      </c>
+      <c r="J28" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" t="s">
+        <v>121</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="7"/>
+        <v>4.5</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="5"/>
+        <v>1.9</v>
+      </c>
+      <c r="H29" t="s">
+        <v>30</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="6"/>
+        <v>42052</v>
+      </c>
+      <c r="J29" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="7"/>
+        <v>6.5</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="5"/>
+        <v>0.8</v>
+      </c>
+      <c r="H30" t="s">
+        <v>31</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="6"/>
+        <v>43531</v>
+      </c>
+      <c r="J30" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="7"/>
+        <v>2.5</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>30</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="6"/>
+        <v>43863</v>
+      </c>
+      <c r="J31" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" t="s">
+        <v>124</v>
+      </c>
+      <c r="E32">
+        <f>E2+5</f>
+        <v>23</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="7"/>
+        <v>1.5</v>
+      </c>
+      <c r="G32">
+        <f>G2+1</f>
+        <v>2.5</v>
+      </c>
+      <c r="H32" t="s">
+        <v>31</v>
+      </c>
+      <c r="I32" s="1">
+        <f t="shared" si="6"/>
+        <v>44174</v>
+      </c>
+      <c r="J32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" t="s">
+        <v>125</v>
+      </c>
+      <c r="E33">
+        <f t="shared" ref="E33:E42" si="8">E3+5</f>
+        <v>28</v>
+      </c>
+      <c r="F33">
+        <f>F2+1.5</f>
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <f t="shared" ref="G33:G42" si="9">G3+1</f>
+        <v>2.7</v>
+      </c>
+      <c r="H33" t="s">
+        <v>31</v>
+      </c>
+      <c r="I33" s="1">
+        <f>I2-360</f>
+        <v>43604</v>
+      </c>
+      <c r="J33" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" t="s">
+        <v>126</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="8"/>
+        <v>40</v>
+      </c>
+      <c r="F34">
+        <f t="shared" ref="F34:F43" si="10">F3+1.5</f>
+        <v>3.5</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="9"/>
+        <v>2.9</v>
+      </c>
+      <c r="H34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I34" s="1">
+        <f t="shared" ref="I34:I43" si="11">I3-360</f>
+        <v>40376</v>
+      </c>
+      <c r="J34" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" t="s">
+        <v>127</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="8"/>
+        <v>47</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="10"/>
+        <v>5.5</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="9"/>
+        <v>2.6</v>
+      </c>
+      <c r="H35" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" s="1">
+        <f t="shared" si="11"/>
+        <v>42540</v>
+      </c>
+      <c r="J35" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36" t="s">
+        <v>128</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="8"/>
+        <v>37</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="10"/>
+        <v>3.5</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="9"/>
+        <v>3.3</v>
+      </c>
+      <c r="H36" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="1">
+        <f t="shared" si="11"/>
+        <v>43424</v>
+      </c>
+      <c r="J36" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" t="s">
+        <v>129</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="8"/>
+        <v>30</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="10"/>
+        <v>9.5</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="9"/>
+        <v>3.1</v>
+      </c>
+      <c r="H37" t="s">
+        <v>30</v>
+      </c>
+      <c r="I37" s="1">
+        <f t="shared" si="11"/>
+        <v>40939</v>
+      </c>
+      <c r="J37" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" t="s">
+        <v>130</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="8"/>
+        <v>34</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="10"/>
+        <v>4.5</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="9"/>
+        <v>2.79</v>
+      </c>
+      <c r="H38" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="1">
+        <f t="shared" si="11"/>
+        <v>42803</v>
+      </c>
+      <c r="J38" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" t="s">
+        <v>131</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="8"/>
+        <v>24</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="10"/>
+        <v>5.5</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="9"/>
+        <v>3.4</v>
+      </c>
+      <c r="H39" t="s">
+        <v>30</v>
+      </c>
+      <c r="I39" s="1">
+        <f t="shared" si="11"/>
+        <v>42522</v>
+      </c>
+      <c r="J39" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40" t="s">
+        <v>132</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="10"/>
+        <v>7.5</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="9"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H40" t="s">
+        <v>31</v>
+      </c>
+      <c r="I40" s="1">
+        <f t="shared" si="11"/>
+        <v>41842</v>
+      </c>
+      <c r="J40" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" t="s">
+        <v>133</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="10"/>
+        <v>3.5</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="9"/>
+        <v>2.5</v>
+      </c>
+      <c r="H41" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" s="1">
+        <f t="shared" si="11"/>
+        <v>43321</v>
+      </c>
+      <c r="J41" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>134</v>
+      </c>
+      <c r="E42">
+        <f>E2+6</f>
+        <v>24</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="10"/>
+        <v>2.5</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="H42" t="s">
+        <v>31</v>
+      </c>
+      <c r="I42" s="1">
+        <f t="shared" si="11"/>
+        <v>43653</v>
+      </c>
+      <c r="J42" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" t="s">
+        <v>135</v>
+      </c>
+      <c r="E43">
+        <f t="shared" ref="E43:E51" si="12">E3+6</f>
+        <v>29</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="G43">
+        <f>G2+2</f>
+        <v>3.5</v>
+      </c>
+      <c r="H43" t="s">
+        <v>31</v>
+      </c>
+      <c r="I43" s="1">
+        <f t="shared" si="11"/>
+        <v>43964</v>
+      </c>
+      <c r="J43" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" t="s">
+        <v>136</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="12"/>
+        <v>41</v>
+      </c>
+      <c r="F44">
+        <f>F2+2</f>
+        <v>2.5</v>
+      </c>
+      <c r="G44">
+        <f t="shared" ref="G44:G51" si="13">G3+2</f>
+        <v>3.7</v>
+      </c>
+      <c r="H44" t="s">
+        <v>31</v>
+      </c>
+      <c r="I44" s="1">
+        <f>I2-720</f>
+        <v>43244</v>
+      </c>
+      <c r="J44" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" t="s">
+        <v>137</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="12"/>
+        <v>48</v>
+      </c>
+      <c r="F45">
+        <f t="shared" ref="F45:F51" si="14">F3+2</f>
+        <v>4</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="13"/>
+        <v>3.9</v>
+      </c>
+      <c r="H45" t="s">
+        <v>31</v>
+      </c>
+      <c r="I45" s="1">
+        <f t="shared" ref="I45:I51" si="15">I3-720</f>
+        <v>40016</v>
+      </c>
+      <c r="J45" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" t="s">
+        <v>138</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="12"/>
+        <v>38</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="13"/>
+        <v>3.6</v>
+      </c>
+      <c r="H46" t="s">
+        <v>30</v>
+      </c>
+      <c r="I46" s="1">
+        <f t="shared" si="15"/>
+        <v>42180</v>
+      </c>
+      <c r="J46" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" t="s">
+        <v>139</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="12"/>
+        <v>31</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="13"/>
+        <v>4.3</v>
+      </c>
+      <c r="H47" t="s">
+        <v>30</v>
+      </c>
+      <c r="I47" s="1">
+        <f t="shared" si="15"/>
+        <v>43064</v>
+      </c>
+      <c r="J47" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" t="s">
+        <v>101</v>
+      </c>
+      <c r="D48" t="s">
+        <v>140</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="12"/>
+        <v>35</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="14"/>
+        <v>10</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="13"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H48" t="s">
+        <v>30</v>
+      </c>
+      <c r="I48" s="1">
+        <f t="shared" si="15"/>
+        <v>40579</v>
+      </c>
+      <c r="J48" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" t="s">
+        <v>100</v>
+      </c>
+      <c r="D49" t="s">
+        <v>141</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="12"/>
+        <v>25</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="13"/>
+        <v>3.79</v>
+      </c>
+      <c r="H49" t="s">
+        <v>30</v>
+      </c>
+      <c r="I49" s="1">
+        <f t="shared" si="15"/>
+        <v>42443</v>
+      </c>
+      <c r="J49" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" t="s">
+        <v>103</v>
+      </c>
+      <c r="D50" t="s">
+        <v>142</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="12"/>
+        <v>30</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="13"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H50" t="s">
+        <v>31</v>
+      </c>
+      <c r="I50" s="1">
+        <f t="shared" si="15"/>
+        <v>42162</v>
+      </c>
+      <c r="J50" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>77</v>
+      </c>
+      <c r="C51" t="s">
+        <v>102</v>
+      </c>
+      <c r="D51" t="s">
+        <v>143</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="12"/>
+        <v>36</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="13"/>
+        <v>3.3</v>
+      </c>
+      <c r="H51" t="s">
+        <v>30</v>
+      </c>
+      <c r="I51" s="1">
+        <f t="shared" si="15"/>
+        <v>41482</v>
+      </c>
+      <c r="J51" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>